<commit_message>
added missing part of the uk statement
</commit_message>
<xml_diff>
--- a/python-service/November_2024.xlsx
+++ b/python-service/November_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codingv2/financial-dashboard/python-service/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EDEE4D8-97D4-E945-9F78-555889BEF4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2BC594-9ECC-B349-924C-9D1DCEF971D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10060" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Balance Statement" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="235">
   <si>
     <t>Date</t>
   </si>
@@ -649,6 +649,96 @@
   </si>
   <si>
     <t>Exchange Rate</t>
+  </si>
+  <si>
+    <t>Sent money to Client AC re Foresight Works</t>
+  </si>
+  <si>
+    <t>Sent money to Foresight Works Ltd</t>
+  </si>
+  <si>
+    <t>Card transaction of 97.61 GBP issued by Chisou Restaurant London</t>
+  </si>
+  <si>
+    <t>Card transaction of 13.00 GBP issued by Zettle_*Stuart Austrie Forest Gate</t>
+  </si>
+  <si>
+    <t>Card transaction of 139.21 GBP issued by Ganymede London</t>
+  </si>
+  <si>
+    <t>Card transaction of 8.99 GBP issued by Amazon.co.uk 3528008547917</t>
+  </si>
+  <si>
+    <t>Sent money to american express</t>
+  </si>
+  <si>
+    <t>Card transaction of 1,602.00 GBP issued by Zendesk.com - Ire +18886704887</t>
+  </si>
+  <si>
+    <t>Card transaction of 613.44 GBP issued by Paypal *Hotels.com 35314369001</t>
+  </si>
+  <si>
+    <t>Card transaction of 17.20 GBP issued by Sumup  *John Hensman Bexleyheath</t>
+  </si>
+  <si>
+    <t>Card transaction of 53.20 GBP issued by Artist Residence London</t>
+  </si>
+  <si>
+    <t>Sent money to mishcon de reya llp</t>
+  </si>
+  <si>
+    <t>Card transaction of 207.83 GBP issued by Slack Tc05m7fbl +35315137661</t>
+  </si>
+  <si>
+    <t>Card transaction of 79.99 GBP issued by Linkedin Sn *192534486 LNKD.IN/BILL</t>
+  </si>
+  <si>
+    <t>Card transaction of 32.80 GBP issued by Lopay  Taxi* Lopay CROYDON</t>
+  </si>
+  <si>
+    <t>Received money from CLP POWER HONG KONG LIMITED with reference INV. 091024 FR.09.10.24 Y1: MODULE 2 (BLUE BELT)</t>
+  </si>
+  <si>
+    <t>Card transaction of 6.20 GBP issued by Tfl Travel Charge TFL.gov.uk/CP</t>
+  </si>
+  <si>
+    <t>Card transaction of 16.40 GBP issued by Cmt Uk Ltd Taxi Fare London</t>
+  </si>
+  <si>
+    <t>Card transaction of 11.40 GBP issued by Txw*London Taxi 61667 Glasgow</t>
+  </si>
+  <si>
+    <t>Card transaction of 24.90 GBP issued by Gails Canary Wharf London</t>
+  </si>
+  <si>
+    <t>Fee refund</t>
+  </si>
+  <si>
+    <t>Card transaction of 5.35 GBP issued by Uber   *Lime London</t>
+  </si>
+  <si>
+    <t>Card transaction of 16.64 GBP issued by Adobe Saggart, Dubl</t>
+  </si>
+  <si>
+    <t>Card transaction of 45.83 GBP issued by Linkedin Pre P276630274 LINKEDIN.COM</t>
+  </si>
+  <si>
+    <t>Card transaction of 14.04 GBP issued by Amznbusiness amazon.co.uk</t>
+  </si>
+  <si>
+    <t>Card transaction of 16.64 GBP issued by Adobe  *Adobe Dublin</t>
+  </si>
+  <si>
+    <t>Card transaction of 15.60 GBP issued by Cmt Uk Ltd Taxi Fare London</t>
+  </si>
+  <si>
+    <t>Card transaction of 152.40 GBP issued by Wheely * C41bc7 London</t>
+  </si>
+  <si>
+    <t>Card transaction of -822.87 GBP issued by Paypal *Hotels.com 35314369001</t>
+  </si>
+  <si>
+    <t>Insurance</t>
   </si>
 </sst>
 </file>
@@ -1034,10 +1124,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:H181"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
-      <selection activeCell="A164" sqref="A164"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="D193" sqref="D193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1531,7 +1621,7 @@
         <v>134</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F24" t="s">
         <v>26</v>
@@ -1551,7 +1641,7 @@
         <v>134</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F25" t="s">
         <v>27</v>
@@ -1571,7 +1661,7 @@
         <v>134</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F26" t="s">
         <v>28</v>
@@ -1611,7 +1701,7 @@
         <v>134</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F28" t="s">
         <v>30</v>
@@ -3045,7 +3135,7 @@
         <v>134</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F100" t="s">
         <v>82</v>
@@ -3185,7 +3275,7 @@
         <v>134</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F107" t="s">
         <v>89</v>
@@ -3950,7 +4040,7 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="3">
-        <v>45626</v>
+        <v>45625</v>
       </c>
       <c r="B146">
         <v>-16017.13</v>
@@ -3970,7 +4060,7 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="3">
-        <v>45627</v>
+        <v>45625</v>
       </c>
       <c r="B147">
         <v>-8540.4599999999991</v>
@@ -3990,7 +4080,7 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="3">
-        <v>45628</v>
+        <v>45625</v>
       </c>
       <c r="B148">
         <v>-7117.97</v>
@@ -4010,7 +4100,7 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="3">
-        <v>45629</v>
+        <v>45625</v>
       </c>
       <c r="B149">
         <v>-4454.4799999999996</v>
@@ -4030,7 +4120,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="3">
-        <v>45630</v>
+        <v>45625</v>
       </c>
       <c r="B150">
         <v>-5111.2299999999996</v>
@@ -4050,7 +4140,7 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="3">
-        <v>45631</v>
+        <v>45625</v>
       </c>
       <c r="B151">
         <v>-9488.7999999999993</v>
@@ -4070,7 +4160,7 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="3">
-        <v>45632</v>
+        <v>45625</v>
       </c>
       <c r="B152">
         <v>-1014.4</v>
@@ -4090,7 +4180,7 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="3">
-        <v>45633</v>
+        <v>45625</v>
       </c>
       <c r="B153">
         <v>16079.72</v>
@@ -4323,7 +4413,9 @@
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A165" s="1"/>
+      <c r="A165" s="1">
+        <v>45625</v>
+      </c>
       <c r="B165">
         <v>-14625.377874372498</v>
       </c>
@@ -4341,6 +4433,9 @@
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A166" s="1">
+        <v>45625</v>
+      </c>
       <c r="B166">
         <v>-13372.901251195279</v>
       </c>
@@ -4358,6 +4453,9 @@
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A167" s="1">
+        <v>45625</v>
+      </c>
       <c r="B167">
         <v>-12778.943651919006</v>
       </c>
@@ -4375,6 +4473,9 @@
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A168" s="1">
+        <v>45625</v>
+      </c>
       <c r="B168">
         <v>-9830.1318532816076</v>
       </c>
@@ -4392,6 +4493,9 @@
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A169" s="1">
+        <v>45625</v>
+      </c>
       <c r="B169">
         <v>-10537.227335115933</v>
       </c>
@@ -4409,6 +4513,9 @@
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A170" s="1">
+        <v>45625</v>
+      </c>
       <c r="B170">
         <v>-9108.6378677116663</v>
       </c>
@@ -4426,6 +4533,9 @@
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171" s="1">
+        <v>45625</v>
+      </c>
       <c r="B171">
         <v>-9522.6649547714933</v>
       </c>
@@ -4443,6 +4553,9 @@
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172" s="1">
+        <v>45625</v>
+      </c>
       <c r="B172">
         <v>-9395.1517526963835</v>
       </c>
@@ -4460,6 +4573,9 @@
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A173" s="1">
+        <v>45625</v>
+      </c>
       <c r="B173">
         <v>-8601.9053707120111</v>
       </c>
@@ -4477,6 +4593,9 @@
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A174" s="1">
+        <v>45625</v>
+      </c>
       <c r="B174">
         <v>-3588.0338246243155</v>
       </c>
@@ -4494,6 +4613,9 @@
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A175" s="1">
+        <v>45625</v>
+      </c>
       <c r="B175">
         <v>-1563.0027345267306</v>
       </c>
@@ -4511,6 +4633,9 @@
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A176" s="1">
+        <v>45625</v>
+      </c>
       <c r="B176">
         <v>-349.69529659992367</v>
       </c>
@@ -4527,7 +4652,10 @@
         <v>197</v>
       </c>
     </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177" s="1">
+        <v>45625</v>
+      </c>
       <c r="B177">
         <v>-2760.0260189417813</v>
       </c>
@@ -4544,7 +4672,10 @@
         <v>198</v>
       </c>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178" s="1">
+        <v>45625</v>
+      </c>
       <c r="B178">
         <v>-8073.0761054047098</v>
       </c>
@@ -4561,7 +4692,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" s="1">
+        <v>45625</v>
+      </c>
       <c r="B179">
         <v>-1248.3597683673677</v>
       </c>
@@ -4578,7 +4712,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" s="1">
+        <v>45625</v>
+      </c>
       <c r="B180">
         <v>-3312.0312227301374</v>
       </c>
@@ -4595,7 +4732,10 @@
         <v>201</v>
       </c>
     </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A181" s="1">
+        <v>45625</v>
+      </c>
       <c r="B181">
         <v>-871.89221938370872</v>
       </c>
@@ -4610,6 +4750,619 @@
       </c>
       <c r="F181" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A182" s="1">
+        <v>45624</v>
+      </c>
+      <c r="B182">
+        <v>-80000</v>
+      </c>
+      <c r="C182" t="s">
+        <v>131</v>
+      </c>
+      <c r="F182" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A183" s="1">
+        <v>45624</v>
+      </c>
+      <c r="B183">
+        <v>80000</v>
+      </c>
+      <c r="C183" t="s">
+        <v>131</v>
+      </c>
+      <c r="F183" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" s="1">
+        <v>45623</v>
+      </c>
+      <c r="B184">
+        <v>-50</v>
+      </c>
+      <c r="C184" t="s">
+        <v>131</v>
+      </c>
+      <c r="F184" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A185" s="1">
+        <v>45623</v>
+      </c>
+      <c r="B185">
+        <v>50</v>
+      </c>
+      <c r="C185" t="s">
+        <v>131</v>
+      </c>
+      <c r="F185" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A186" s="1">
+        <v>45616</v>
+      </c>
+      <c r="B186">
+        <v>-2147.15</v>
+      </c>
+      <c r="C186" t="s">
+        <v>131</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E186" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F186" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187" s="1">
+        <v>45615</v>
+      </c>
+      <c r="B187">
+        <v>-97.61</v>
+      </c>
+      <c r="C187" t="s">
+        <v>131</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E187" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F187" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A188" s="1">
+        <v>45614</v>
+      </c>
+      <c r="B188">
+        <v>-13</v>
+      </c>
+      <c r="C188" t="s">
+        <v>131</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E188" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F188" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" s="1">
+        <v>45614</v>
+      </c>
+      <c r="B189">
+        <v>-139.21</v>
+      </c>
+      <c r="C189" t="s">
+        <v>131</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F189" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" s="1">
+        <v>45614</v>
+      </c>
+      <c r="B190">
+        <v>-8.99</v>
+      </c>
+      <c r="C190" t="s">
+        <v>131</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F190" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" s="1">
+        <v>45614</v>
+      </c>
+      <c r="B191">
+        <v>-1500</v>
+      </c>
+      <c r="C191" t="s">
+        <v>131</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F191" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" s="1">
+        <v>45612</v>
+      </c>
+      <c r="B192">
+        <v>-1602</v>
+      </c>
+      <c r="C192" t="s">
+        <v>131</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E192" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F192" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A193" s="1">
+        <v>45612</v>
+      </c>
+      <c r="B193">
+        <v>-613.44000000000005</v>
+      </c>
+      <c r="C193" t="s">
+        <v>131</v>
+      </c>
+      <c r="D193" s="2"/>
+      <c r="F193" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194" s="1">
+        <v>45611</v>
+      </c>
+      <c r="B194">
+        <v>-17.2</v>
+      </c>
+      <c r="C194" t="s">
+        <v>131</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E194" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F194" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195" s="1">
+        <v>45611</v>
+      </c>
+      <c r="B195">
+        <v>-53.2</v>
+      </c>
+      <c r="C195" t="s">
+        <v>131</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E195" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F195" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A196" s="1">
+        <v>45611</v>
+      </c>
+      <c r="B196">
+        <v>-154200</v>
+      </c>
+      <c r="C196" t="s">
+        <v>131</v>
+      </c>
+      <c r="D196" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E196" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F196" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A197" s="1">
+        <v>45611</v>
+      </c>
+      <c r="B197">
+        <v>120000</v>
+      </c>
+      <c r="C197" t="s">
+        <v>131</v>
+      </c>
+      <c r="F197" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A198" s="1">
+        <v>45611</v>
+      </c>
+      <c r="B198">
+        <v>-207.83</v>
+      </c>
+      <c r="C198" t="s">
+        <v>131</v>
+      </c>
+      <c r="D198" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E198" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F198" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A199" s="1">
+        <v>45609</v>
+      </c>
+      <c r="B199">
+        <v>-79.989999999999995</v>
+      </c>
+      <c r="C199" t="s">
+        <v>131</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E199" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F199" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A200" s="1">
+        <v>45609</v>
+      </c>
+      <c r="B200">
+        <v>-32.799999999999997</v>
+      </c>
+      <c r="C200" t="s">
+        <v>131</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E200" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F200" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A201" s="1">
+        <v>45608</v>
+      </c>
+      <c r="B201">
+        <v>39985</v>
+      </c>
+      <c r="C201" t="s">
+        <v>131</v>
+      </c>
+      <c r="F201" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A202" s="1">
+        <v>45608</v>
+      </c>
+      <c r="B202">
+        <v>-6.2</v>
+      </c>
+      <c r="C202" t="s">
+        <v>131</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E202" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F202" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A203" s="1">
+        <v>45607</v>
+      </c>
+      <c r="B203">
+        <v>-16.399999999999999</v>
+      </c>
+      <c r="C203" t="s">
+        <v>131</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F203" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A204" s="1">
+        <v>45607</v>
+      </c>
+      <c r="B204">
+        <v>-11.4</v>
+      </c>
+      <c r="C204" t="s">
+        <v>131</v>
+      </c>
+      <c r="D204" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E204" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F204" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A205" s="1">
+        <v>45607</v>
+      </c>
+      <c r="B205">
+        <v>-24.9</v>
+      </c>
+      <c r="C205" t="s">
+        <v>131</v>
+      </c>
+      <c r="D205" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E205" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F205" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A206" s="1">
+        <v>45607</v>
+      </c>
+      <c r="B206">
+        <v>229.95</v>
+      </c>
+      <c r="C206" t="s">
+        <v>131</v>
+      </c>
+      <c r="F206" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A207" s="1">
+        <v>45607</v>
+      </c>
+      <c r="B207">
+        <v>-5.35</v>
+      </c>
+      <c r="C207" t="s">
+        <v>131</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E207" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F207" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A208" s="1">
+        <v>45606</v>
+      </c>
+      <c r="B208">
+        <v>-16.64</v>
+      </c>
+      <c r="C208" t="s">
+        <v>131</v>
+      </c>
+      <c r="D208" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E208" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F208" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A209" s="1">
+        <v>45606</v>
+      </c>
+      <c r="B209">
+        <v>-45.83</v>
+      </c>
+      <c r="C209" t="s">
+        <v>131</v>
+      </c>
+      <c r="D209" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E209" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F209" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A210" s="1">
+        <v>45606</v>
+      </c>
+      <c r="B210">
+        <v>-14.04</v>
+      </c>
+      <c r="C210" t="s">
+        <v>131</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E210" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F210" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A211" s="1">
+        <v>45604</v>
+      </c>
+      <c r="B211">
+        <v>-16.64</v>
+      </c>
+      <c r="C211" t="s">
+        <v>131</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E211" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F211" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A212" s="1">
+        <v>45604</v>
+      </c>
+      <c r="B212">
+        <v>-15.6</v>
+      </c>
+      <c r="C212" t="s">
+        <v>131</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E212" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F212" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A213" s="1">
+        <v>45604</v>
+      </c>
+      <c r="B213">
+        <v>-152.4</v>
+      </c>
+      <c r="C213" t="s">
+        <v>131</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E213" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F213" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A214" s="1">
+        <v>45604</v>
+      </c>
+      <c r="B214">
+        <v>822.87</v>
+      </c>
+      <c r="C214" t="s">
+        <v>131</v>
+      </c>
+      <c r="D214" s="2"/>
+      <c r="F214" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="1048576" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1048576" s="1">
+        <v>45625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>